<commit_message>
Update RECU Altium project
</commit_message>
<xml_diff>
--- a/ETRX_RECU/ETRX_RECU.xlsx
+++ b/ETRX_RECU/ETRX_RECU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9068b3d81be815ab/download/New/download/Documentos/GitHub/ADCAN/ETRX_RECU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_AD4D2F04E46CFB4ACB3E201215D3DB9A693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7CE3A35-7694-4619-842E-A306B44894EA}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="11_AD4D2F04E46CFB4ACB3E201215D3DB9A693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6CB48E5-8DE3-49B9-AAE5-6F3B15A69E92}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="2805" windowWidth="18780" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Susp_R_L</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>1 digital</t>
-  </si>
-  <si>
-    <t>Refri_Inverters</t>
   </si>
   <si>
     <t>Tyre_temperatuae</t>
@@ -137,7 +134,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -198,7 +195,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -214,10 +211,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,10 +542,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2">
         <v>3.3</v>
@@ -565,13 +558,13 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2">
         <v>4</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -672,84 +665,72 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2">
+        <v>400</v>
+      </c>
+      <c r="E11" s="3">
+        <f>(D11/C11)*1000</f>
+        <v>16666.666666666668</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2">
         <v>24</v>
       </c>
       <c r="D12" s="2">
-        <v>200</v>
-      </c>
-      <c r="E12" s="3">
-        <f>(D12/C12)*1000</f>
-        <v>8333.3333333333339</v>
+        <v>120</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" ref="E12:E13" si="0">(D12/C12)*1000</f>
+        <v>5000</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2">
         <v>24</v>
       </c>
       <c r="D13" s="2">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" ref="E13:E14" si="0">(D13/C13)*1000</f>
-        <v>5000</v>
+        <f t="shared" si="0"/>
+        <v>8333.3333333333339</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2">
-        <v>24</v>
-      </c>
-      <c r="D14" s="2">
-        <v>150</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>6250</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>